<commit_message>
Updated chrom position of one cpg
</commit_message>
<xml_diff>
--- a/Results/DMPs_and_DMRs.xlsx
+++ b/Results/DMPs_and_DMRs.xlsx
@@ -13060,22 +13060,22 @@
         <v>13</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0000000000000000000000000000102702340304089</v>
+        <v>0.0000000000000000000000000000102707141083333</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00000004063967942483</v>
+        <v>0.0000000406405368585784</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0550280645262266</v>
+        <v>0.0550282766040125</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00000464694620319481</v>
+        <v>0.00000464704173680665</v>
       </c>
       <c r="K2" t="n">
         <v>0.0808076008801439</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0666336886416738</v>
+        <v>0.0666337225406583</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -13156,16 +13156,16 @@
         <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00000000000000000000000000059631364291328</v>
+        <v>0.000000000000000000000000000596335584544442</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0251041149838138</v>
+        <v>0.0251047265141457</v>
       </c>
       <c r="I2" t="n">
-        <v>0.117175981040224</v>
+        <v>0.117176238982109</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0568270018269931</v>
+        <v>0.0568278351748385</v>
       </c>
       <c r="K2" t="n">
         <v>0.0703450858843091</v>
@@ -13252,22 +13252,22 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0000000000000000000000000000330459005018972</v>
+        <v>0.0000000000000000000000000000330469954705397</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0583279109111943</v>
+        <v>0.0583277095659426</v>
       </c>
       <c r="I2" t="n">
-        <v>0.235054182864396</v>
+        <v>0.235054052598167</v>
       </c>
       <c r="J2" t="n">
-        <v>0.186263105822191</v>
+        <v>0.186262664276511</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0502441957064725</v>
+        <v>0.0502391934248481</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0352847487006647</v>
+        <v>0.0352827141650306</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -13348,22 +13348,22 @@
         <v>13</v>
       </c>
       <c r="G2" t="n">
-        <v>0.000000000000000000000000000506789037512438</v>
+        <v>0.000000000000000000000000000506809247461483</v>
       </c>
       <c r="H2" t="n">
-        <v>0.000000219792566883217</v>
+        <v>0.000000219797221054187</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0664963720956521</v>
+        <v>0.0664966134439882</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0000196562210716002</v>
+        <v>0.0000196566147978176</v>
       </c>
       <c r="K2" t="n">
         <v>0.0797069041402041</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0656024838782411</v>
+        <v>0.0656025119025866</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>

</xml_diff>

<commit_message>
repeated analyses for ctq
</commit_message>
<xml_diff>
--- a/Results/DMPs_and_DMRs.xlsx
+++ b/Results/DMPs_and_DMRs.xlsx
@@ -15,6 +15,8 @@
     <sheet name="DMR_group_ageControlled" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="T-tests_Group" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="LinearModels_GeneExpr" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="DMPs_ctq" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="DMR_ctq" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
@@ -5281,6 +5283,3957 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.00138168201444347</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0141818181818182</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.65893453756403</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.000000122393192679175</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.000020317269984743</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.55611078592651</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.00194222612815712</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0177272727272727</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.20827656756791</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0000527242415959223</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00437611205246155</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-2.34021053853579</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.000489473080891063</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0291818181818182</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3.10271247137727</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.00243708689866629</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.109716612886358</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-5.96901043741281</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.00202323182148179</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0720909090909091</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.07640585640061</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.00264377380449055</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.109716612886358</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-6.04447790301419</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.000710710328225898</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0161818181818182</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.90255293134766</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.00447242739112107</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.125022987672004</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-6.52950577574827</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.00120400443238699</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0368181818181818</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.89906149778064</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.00451890316886763</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.125022987672004</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-6.53899973413213</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.00143937946582095</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0660909090909091</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.84316949946922</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0053258522064568</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.126298780895976</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-6.68964350182627</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.000320583852355661</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0157272727272727</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2.66150890900925</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.00894383126384739</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.185584498724833</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-7.16164966116676</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.000363379312980016</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0179090909090909</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.60420613999114</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0104800149460893</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.193298053450092</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-7.30486693104669</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.000966718887318023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0356363636363636</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.54955711504531</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0121626740196402</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.201900388726028</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-7.43888199880942</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.000390508578197241</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0181818181818182</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.45662248448769</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0155876737110945</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.235232166912881</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-7.66096910508522</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.00121890642314012</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0741818181818182</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.34942629621398</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.020585953852579</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.279414845583426</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-7.90793748357778</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.00160482977341332</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.153090909090909</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.28128858276015</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0244560547895446</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.279414845583426</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-8.05973662079807</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.000976653547820106</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0745454545454545</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.27066561515996</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.025113793029489</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.279414845583426</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-8.08303696966439</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.000468075350578885</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0491818181818182</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.26852288342329</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0252483294201891</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.279414845583426</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-8.08772482469847</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.000144816781934202</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.17557724400027</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0317260870065115</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.329158152692557</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-8.28717719545451</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.0010484887852967</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.144909090909091</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.08221067501533</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0396417176065514</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.387089713099266</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-8.47981224636544</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.000411906308509419</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0890909090909091</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.02747047803653</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0450309662197032</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.415285577359485</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-8.58912113410178</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.000292690382484429</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0343636363636364</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.98429685730997</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0497121870782177</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.422524836427302</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-8.67342596980542</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.000431011424859577</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0636363636363636</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.97383741739549</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0509066067984701</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.422524836427302</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-8.69359596931605</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.000490619387872072</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0305454545454545</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.86769579195372</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0644651994893625</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.468024271343084</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-8.89264241421002</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.000538382178747468</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0155454545454545</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.85213468968097</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0666868423265579</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.468024271343084</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-8.92095744796779</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.000248748614879065</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0186363636363636</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.85008739269169</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0669838355011012</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.468024271343084</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-8.92466615175328</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.0015177104428566</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0349090909090909</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.8328407491387</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0695298072610105</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.468024271343084</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-8.95575558191469</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.000364525619961025</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.81307882274434</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0725455890513956</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.468024271343084</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-8.99104226990346</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.000278170494058309</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0236363636363636</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.8082102116383</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0733050063549409</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.468024271343084</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-8.99968029805624</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.00122272744641015</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0407272727272727</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.69498945021767</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0929054900302828</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.568153959417704</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-9.19436521731605</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.000405792671277367</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.107636363636364</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.67835443814382</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0961157443902076</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.568153959417704</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-9.2219643031298</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.00117687516716977</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.674727272727273</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.6625136344606</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0992558121874303</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.568153959417704</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-9.2480052813201</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.000235375033433953</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0218181818181818</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.61843666992602</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.108431336928179</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.591941274407517</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-9.3192270036897</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.000186083833250545</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0126363636363636</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.59387460394029</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.113832488890593</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.591941274407517</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-9.3581238482413</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.000404646364296358</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.59264171178497</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.11410916133157</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.591941274407517</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-9.36006130853285</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.000252569638149096</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0335454545454545</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.57504484570422</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.118116830851091</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.594163452160035</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-9.38755823952651</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.000390508578197241</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.0605454545454545</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.55410848673511</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.123029977520615</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.600675772600649</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-9.41989292971558</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.000175384968094456</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.0175454545454545</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-1.53576135366191</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.127467281259171</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.60455910540064</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-9.44788822563541</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.000884566887012342</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.49632308567139</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.137432157890313</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.633714950271997</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-9.50698671975723</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.000537617974093462</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0137272727272727</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.47872387340115</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.142071004680838</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.637399642622138</v>
+      </c>
+      <c r="G38" t="n">
+        <v>-9.53288296444666</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.000759619426082303</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.232363636363636</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1.4641565167715</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.14600215600251</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.637798892010965</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-9.55409524438764</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.000719880784073975</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.40950841913637</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.161504801089805</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.687430691818144</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-9.63186885863913</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.000200603721676665</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0537272727272727</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.35867720277666</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.177027498059323</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.734664116946191</v>
+      </c>
+      <c r="G41" t="n">
+        <v>-9.70164772764678</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.000828779947269879</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.3353017572499</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.18453327004065</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.747134703091414</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-9.73290474283612</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.000872721714875243</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.461454545454545</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.28368583294631</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.201948434215907</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.77248842218707</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-9.80006238695534</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.000453555462152765</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.117545454545455</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.27194950483225</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.206072558383515</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.77248842218707</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-9.81497419978522</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.000700393565396813</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.227181818181818</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.26423110768772</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.208818387025777</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.77248842218707</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-9.82470846135192</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.000234992931106951</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.0859090909090909</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.26257925196607</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.209409512038664</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.77248842218707</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-9.82678426688375</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.000697718849107789</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.252545454545455</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.22534431036116</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.223061758132707</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.804961996739767</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-9.87287546437268</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="n">
+        <v>-0.000324022773298689</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.920727272727273</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-1.20386845881361</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.231223708265961</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.816311311085238</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-9.89884882200896</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.000636200374460279</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.203545454545455</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.19144636843932</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.236041824892117</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.816311311085238</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-9.91366816617984</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.000177677582056475</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.0577272727272727</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.17254961252256</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.243508597008607</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.819129908099235</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-9.93592434958996</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.000209009972870735</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.0119090909090909</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.15599848873513</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.250185451434318</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.819129908099235</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-9.9551327668324</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.000639639295403308</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.252727272727273</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.13271054192716</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.25979787903415</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.819129908099235</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-9.98170816196979</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.000459286997057811</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.113090909090909</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.1317737435412</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.260189906704859</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.819129908099235</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-9.98276615175597</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.000586144969622865</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.208727272727273</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1.11704664139631</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.266407430204579</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.819129908099235</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-9.9992860301835</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.00068319896068167</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.324545454545455</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1.11691388270418</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.266463946008185</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.819129908099235</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-9.99943398817622</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.000657980207099462</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.511636363636364</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.09578066335465</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.275567210943872</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.831711945757867</v>
+      </c>
+      <c r="G56" t="n">
+        <v>-10.0227674369438</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="n">
+        <v>-0.000258683275381147</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.0117272727272727</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-1.07204376464271</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.286045893692405</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.847921756302487</v>
+      </c>
+      <c r="G57" t="n">
+        <v>-10.0484555155303</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.000622062588361164</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.278363636363636</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.0603425048159</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.291310610392533</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.848378268862463</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-10.060915894393</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.000181498605326506</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0546363636363636</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.04726620165442</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.297271680517778</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.850812051137088</v>
+      </c>
+      <c r="G59" t="n">
+        <v>-10.0746819743519</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.000621298383707156</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.506363636363636</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.02656381533635</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.306877208464771</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.863417230595797</v>
+      </c>
+      <c r="G60" t="n">
+        <v>-10.096133917143</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" t="n">
+        <v>-0.000162775591303351</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.0161818181818182</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-1.01008673146902</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.314669639153664</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.863542707843435</v>
+      </c>
+      <c r="G61" t="n">
+        <v>-10.11290725298</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>158</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.000513927629819266</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.0375454545454545</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.996850324900608</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.321024173382144</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.863542707843435</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-10.1261886565214</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.000432539834167589</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.168363636363636</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.993743353503276</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.322527999315018</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.863542707843435</v>
+      </c>
+      <c r="G63" t="n">
+        <v>-10.1292812585783</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="n">
+        <v>-0.000262122196324174</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.0190909090909091</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-0.933411648638532</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.352651089420828</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.921975395937469</v>
+      </c>
+      <c r="G64" t="n">
+        <v>-10.1874521878643</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.000303771349967521</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.0553636363636364</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.916253822464288</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.36153741785645</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.921975395937469</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-10.2033409070315</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.000178441786710481</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.0424545454545455</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.894013489836616</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.373265849352788</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.921975395937469</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-10.2235040592126</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" t="n">
+        <v>-0.0000997287073478278</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.00227272727272727</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-0.893315508490097</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.373637753968281</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.921975395937469</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-10.2241289499195</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>167</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.000235375033433954</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.185454545454545</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.886336896906124</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.37736893097929</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.921975395937469</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-10.2303503300509</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.0000813877956516755</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.0119090909090909</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.885763250735695</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.377676668215349</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.921975395937469</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-10.2308595919794</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.000351534140842916</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.163636363636364</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.83294915586161</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.406677624710196</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.958206869072297</v>
+      </c>
+      <c r="G70" t="n">
+        <v>-10.2763523024216</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.000130678995835085</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.0321818181818182</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.826497245849785</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.410310578779403</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.958206869072297</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-10.2817206327221</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.000131825302816094</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.0344545454545455</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.813254985894336</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.417828026381558</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.958206869072297</v>
+      </c>
+      <c r="G72" t="n">
+        <v>-10.292609723612</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.000471896373848915</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.256636363636364</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.812867056099112</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.418049481774802</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.958206869072297</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-10.2929260980481</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>171</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-0.0000897940468457454</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.0268181818181818</v>
+      </c>
+      <c r="D74" t="n">
+        <v>-0.807047384519553</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.421380129170347</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.958206869072297</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-10.2976544020848</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.00043253983416759</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.282363636363636</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.760105100225839</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.448817243803513</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-10.334565177212</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.000223911963623858</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.00890909090909091</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.729771877291937</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.467080280527902</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-10.3572523176595</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>113</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.000278170494058309</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.148727272727273</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.725040364187928</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.469966239259209</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G77" t="n">
+        <v>-10.3607086861889</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0004336861411486</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.387181818181818</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.720912792589279</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.472491962604633</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-10.3637056888439</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0000917045584807611</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.0187272727272727</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.718509154659238</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.473966269100861</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G79" t="n">
+        <v>-10.3654431454822</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.000282373619655343</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.161909090909091</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.71275685008253</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.477504913872821</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-10.3695778264221</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>146</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.0000974360933858087</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.0208181818181818</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.708328075985491</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.480239315070647</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G81" t="n">
+        <v>-10.3727387345133</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-0.000618241565091131</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.0392727272727273</v>
+      </c>
+      <c r="D82" t="n">
+        <v>-0.675860764458033</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.500546987106367</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G82" t="n">
+        <v>-10.3953149238211</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>147</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.000249894921860074</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.874</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.673957250335555</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.501751761103276</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G83" t="n">
+        <v>-10.3966059458164</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>25</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.000445531313285698</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.499090909090909</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.671513352897382</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.503300833393883</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G84" t="n">
+        <v>-10.398258177779</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>161</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-0.000335103740781781</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.0420909090909091</v>
+      </c>
+      <c r="D85" t="n">
+        <v>-0.650868520267532</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.516488154260704</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G85" t="n">
+        <v>-10.4119778016283</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.000108134958541897</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.0315454545454545</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.648561710105664</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.517972875293952</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G86" t="n">
+        <v>-10.413484402888</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>64</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.0001566619540713</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.0881818181818182</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.648397232806789</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.518078822419156</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G87" t="n">
+        <v>-10.4135916219515</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.000114248595773948</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.0373636363636364</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.61244023473813</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.541510056183456</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G88" t="n">
+        <v>-10.4363830693569</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>31</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.000361850903672003</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.382272727272727</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.602628377310063</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.547995831956844</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G89" t="n">
+        <v>-10.4423781357483</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>155</v>
+      </c>
+      <c r="B90" t="n">
+        <v>-0.000280081005693325</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.181545454545455</v>
+      </c>
+      <c r="D90" t="n">
+        <v>-0.58777515164038</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.55788750001652</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G90" t="n">
+        <v>-10.4512704576922</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91" t="n">
+        <v>-0.0000779488747086471</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.0229090909090909</v>
+      </c>
+      <c r="D91" t="n">
+        <v>-0.587662808323392</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.557962650532008</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G91" t="n">
+        <v>-10.4513368751405</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.000290015666195406</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.196636363636364</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.583842895799416</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.560520894415097</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G92" t="n">
+        <v>-10.453587702164</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>54</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.000550609453211569</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.0640909090909091</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.579969919461337</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.563120541949815</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G93" t="n">
+        <v>-10.4558549027493</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.000103167628290856</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.00709090909090909</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.570588205185412</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.569442131590627</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G94" t="n">
+        <v>-10.461284690283</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-0.000197164800733636</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.0832727272727273</v>
+      </c>
+      <c r="D95" t="n">
+        <v>-0.565471264819354</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.572904441478907</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G95" t="n">
+        <v>-10.4642090861877</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-0.000717588170111956</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.0652727272727273</v>
+      </c>
+      <c r="D96" t="n">
+        <v>-0.547547751693958</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.585111347652154</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G96" t="n">
+        <v>-10.4742460223383</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.000269764242864239</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.199272727272727</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.516149323489341</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.60678574420011</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G97" t="n">
+        <v>-10.4910536455798</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>148</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-0.000296511405754461</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-0.514422891681177</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.607987986574278</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G98" t="n">
+        <v>-10.4919491702027</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>75</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.0000676321118795612</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.0208181818181818</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.491083211856435</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.624345579811641</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G99" t="n">
+        <v>-10.50376268106</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-0.000146345191242214</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.941727272727273</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-0.490776693898504</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.624561680595391</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G100" t="n">
+        <v>-10.5039141946634</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>130</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.000216652019410798</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.796636363636364</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.48888387551039</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.625896876911464</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G101" t="n">
+        <v>-10.5048477391024</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>138</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.000115012800427955</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.0482727272727273</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.47242536590316</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.637558796282991</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G102" t="n">
+        <v>-10.5128137124935</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>132</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.0000477627908753962</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.0266363636363636</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.465335099738245</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.642611105542998</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G103" t="n">
+        <v>-10.5161617008446</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.000145580986588208</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.119909090909091</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.453227470046796</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.651277402107894</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G104" t="n">
+        <v>-10.5217622724392</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>52</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.000167742921554392</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.157727272727273</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.450872140741558</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.652968892016159</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G105" t="n">
+        <v>-10.5228346766151</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-0.000224294065950862</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.0408181818181818</v>
+      </c>
+      <c r="D106" t="n">
+        <v>-0.450514333706281</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.653226011255883</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G106" t="n">
+        <v>-10.5229971025297</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.000274349470788277</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.414727272727273</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.449041098092396</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.654285114236033</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G107" t="n">
+        <v>-10.5236645218787</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>166</v>
+      </c>
+      <c r="B108" t="n">
+        <v>-0.000206335256581713</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.449090909090909</v>
+      </c>
+      <c r="D108" t="n">
+        <v>-0.407655147682885</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.684318878462721</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G108" t="n">
+        <v>-10.5415232657118</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>121</v>
+      </c>
+      <c r="B109" t="n">
+        <v>-0.000115012800427955</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.917545454545455</v>
+      </c>
+      <c r="D109" t="n">
+        <v>-0.39773051214362</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.691599353349952</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G109" t="n">
+        <v>-10.5455502058275</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>43</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.000162393488976347</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.178818181818182</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.397155873262344</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.692021789137752</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G110" t="n">
+        <v>-10.5457803359286</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>70</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.000297275610408467</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.396351966245576</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.692612930419802</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G111" t="n">
+        <v>-10.5461017260769</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>157</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.000111955981811929</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.393955195923466</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.694376485835709</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G112" t="n">
+        <v>-10.5470560654561</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>82</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-0.000100492912001834</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.0771818181818182</v>
+      </c>
+      <c r="D113" t="n">
+        <v>-0.392818857742025</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.695213196230522</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G113" t="n">
+        <v>-10.5475065123862</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>159</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.000058461656031485</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.0273636363636364</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.383654331017251</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.701974916856636</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G114" t="n">
+        <v>-10.551091917999</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>62</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0.000194872186771617</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.739818181818182</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.381534147663892</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.703542655137414</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G115" t="n">
+        <v>-10.551909367345</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.0000588437583584886</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.0314545454545455</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.361909828516127</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.718113458439587</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G116" t="n">
+        <v>-10.5592611693808</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>123</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-0.00025906537770815</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.0290909090909091</v>
+      </c>
+      <c r="D117" t="n">
+        <v>-0.352179076050519</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.725377542234862</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G117" t="n">
+        <v>-10.5627629756814</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>41</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0.000136792633067135</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.147636363636364</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.348317031819867</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.728267590214549</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G118" t="n">
+        <v>-10.5641264137271</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>139</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-0.000300332429024493</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.902181818181818</v>
+      </c>
+      <c r="D119" t="n">
+        <v>-0.346235400858131</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.729826946793085</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G119" t="n">
+        <v>-10.5648550812226</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>46</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0.000161247181995338</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.342154096371868</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.732887548953089</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G120" t="n">
+        <v>-10.5662710779238</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>50</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0.000143288372626188</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0.169181818181818</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.339233522599546</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0.735080359100117</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G121" t="n">
+        <v>-10.5672740778228</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>98</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0.000244163386955026</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.0280909090909091</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.330547619314391</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.741614747561324</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G122" t="n">
+        <v>-10.570206333034</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>61</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0.000210156279851745</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0.519818181818182</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.319920059497937</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.749635559485776</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G123" t="n">
+        <v>-10.57369081514</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>110</v>
+      </c>
+      <c r="B124" t="n">
+        <v>-0.000436742959764626</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0.111727272727273</v>
+      </c>
+      <c r="D124" t="n">
+        <v>-0.311400180343368</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.756085594474821</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G124" t="n">
+        <v>-10.5764021698634</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>143</v>
+      </c>
+      <c r="B125" t="n">
+        <v>-0.000107752856214895</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.0129090909090909</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-0.310276225044219</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.756937791864629</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G125" t="n">
+        <v>-10.5767544016926</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>118</v>
+      </c>
+      <c r="B126" t="n">
+        <v>0.0000362997210653014</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0.0162727272727273</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.307245812294532</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.759236980381315</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G126" t="n">
+        <v>-10.5776977552395</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>78</v>
+      </c>
+      <c r="B127" t="n">
+        <v>-0.000141759963318177</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0.719909090909091</v>
+      </c>
+      <c r="D127" t="n">
+        <v>-0.300908952458395</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.764051742053035</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G127" t="n">
+        <v>-10.5796405178844</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>125</v>
+      </c>
+      <c r="B128" t="n">
+        <v>-0.0000439417676053646</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0.00372727272727273</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-0.296196771102011</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0.767638085598361</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G128" t="n">
+        <v>-10.5810589805407</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>144</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0.0000683963165335683</v>
+      </c>
+      <c r="C129" t="n">
+        <v>0.935727272727273</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0.294674841532314</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0.768797477208385</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G129" t="n">
+        <v>-10.581512336864</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>140</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0.000049673302510412</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0.0287272727272727</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0.293896004149186</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0.769390991185217</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G130" t="n">
+        <v>-10.581743437004</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>69</v>
+      </c>
+      <c r="B131" t="n">
+        <v>0.0000863551259027163</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.104909090909091</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0.277148406169384</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0.782186115423497</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G131" t="n">
+        <v>-10.5865650999491</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>35</v>
+      </c>
+      <c r="B132" t="n">
+        <v>0.000142906270299186</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0.708909090909091</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0.267504117471336</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0.789581779624206</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G132" t="n">
+        <v>-10.5892135596901</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>137</v>
+      </c>
+      <c r="B133" t="n">
+        <v>-0.000130296893508081</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0.0344545454545455</v>
+      </c>
+      <c r="D133" t="n">
+        <v>-0.266719145879195</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0.790184586852528</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G133" t="n">
+        <v>-10.5894250018442</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>66</v>
+      </c>
+      <c r="B134" t="n">
+        <v>0.0000966718887318019</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0.139545454545455</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0.25047176963997</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0.802689585888725</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G134" t="n">
+        <v>-10.5936620789069</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0.0000936150701157769</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0.129181818181818</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0.249785118130748</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0.803219230504465</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G135" t="n">
+        <v>-10.5938352912924</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>169</v>
+      </c>
+      <c r="B136" t="n">
+        <v>-0.0000565511443964694</v>
+      </c>
+      <c r="C136" t="n">
+        <v>0.0118181818181818</v>
+      </c>
+      <c r="D136" t="n">
+        <v>-0.240615070635667</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0.810301181945148</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G136" t="n">
+        <v>-10.596102968565</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>162</v>
+      </c>
+      <c r="B137" t="n">
+        <v>0.000127622177219059</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0.0296363636363636</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0.22897617165009</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0.819312454049938</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G137" t="n">
+        <v>-10.5988591675649</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>42</v>
+      </c>
+      <c r="B138" t="n">
+        <v>0.0000687784188605705</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0.107454545454545</v>
+      </c>
+      <c r="D138" t="n">
+        <v>0.226845023092833</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0.820965130755226</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G138" t="n">
+        <v>-10.5993490587427</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>51</v>
+      </c>
+      <c r="B139" t="n">
+        <v>0.000129914791181078</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.210363636363636</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0.219393503771657</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.826749971912682</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G139" t="n">
+        <v>-10.6010259764433</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>149</v>
+      </c>
+      <c r="B140" t="n">
+        <v>0.00010125711665584</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0.21202911534459</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.832476551831585</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G140" t="n">
+        <v>-10.6026283075998</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>53</v>
+      </c>
+      <c r="B141" t="n">
+        <v>0.0000787130793626535</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="D141" t="n">
+        <v>0.209584894447647</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0.834379198268848</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G141" t="n">
+        <v>-10.6031480360197</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>85</v>
+      </c>
+      <c r="B142" t="n">
+        <v>0.0000389744373543234</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.101454545454545</v>
+      </c>
+      <c r="D142" t="n">
+        <v>0.206101806815651</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0.837092222641809</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G142" t="n">
+        <v>-10.6038782605195</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>34</v>
+      </c>
+      <c r="B143" t="n">
+        <v>0.0000271292652172251</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0.0293636363636364</v>
+      </c>
+      <c r="D143" t="n">
+        <v>0.202712533481492</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0.839734060619524</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G143" t="n">
+        <v>-10.6045770786652</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>156</v>
+      </c>
+      <c r="B144" t="n">
+        <v>-0.0000832983072866917</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0.0265454545454545</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-0.186211026607624</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0.852622120017735</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G144" t="n">
+        <v>-10.6078140191007</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>131</v>
+      </c>
+      <c r="B145" t="n">
+        <v>-0.00003973864200833</v>
+      </c>
+      <c r="C145" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="D145" t="n">
+        <v>-0.185384817035671</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0.853268489094516</v>
+      </c>
+      <c r="F145" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G145" t="n">
+        <v>-10.607968872658</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>44</v>
+      </c>
+      <c r="B146" t="n">
+        <v>0.000214741507775782</v>
+      </c>
+      <c r="C146" t="n">
+        <v>0.0805454545454545</v>
+      </c>
+      <c r="D146" t="n">
+        <v>0.184573693166777</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0.853903153325433</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G146" t="n">
+        <v>-10.6081202293118</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>60</v>
+      </c>
+      <c r="B147" t="n">
+        <v>0.0000473806885483929</v>
+      </c>
+      <c r="C147" t="n">
+        <v>0.0916363636363636</v>
+      </c>
+      <c r="D147" t="n">
+        <v>0.169721448326226</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0.86554083061599</v>
+      </c>
+      <c r="F147" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G147" t="n">
+        <v>-10.6107744044938</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>153</v>
+      </c>
+      <c r="B148" t="n">
+        <v>-0.000017576707042146</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0.0116363636363636</v>
+      </c>
+      <c r="D148" t="n">
+        <v>-0.169707541292061</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0.865551741939249</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G148" t="n">
+        <v>-10.6107767855308</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>88</v>
+      </c>
+      <c r="B149" t="n">
+        <v>-0.0000565511443964694</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0.111636363636364</v>
+      </c>
+      <c r="D149" t="n">
+        <v>-0.168283669811188</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0.866669034731949</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G149" t="n">
+        <v>-10.6110195358641</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>73</v>
+      </c>
+      <c r="B150" t="n">
+        <v>-0.0000611363723205074</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0.143090909090909</v>
+      </c>
+      <c r="D150" t="n">
+        <v>-0.16784325051612</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0.867014680626623</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0.965935818684694</v>
+      </c>
+      <c r="G150" t="n">
+        <v>-10.6110942073016</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>92</v>
+      </c>
+      <c r="B151" t="n">
+        <v>0.000118833823697986</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0.495181818181818</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0.152468729356212</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0.879096463571439</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0.968370994025505</v>
+      </c>
+      <c r="G151" t="n">
+        <v>-10.6135783106822</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>76</v>
+      </c>
+      <c r="B152" t="n">
+        <v>0.0000538764281074475</v>
+      </c>
+      <c r="C152" t="n">
+        <v>0.145545454545455</v>
+      </c>
+      <c r="D152" t="n">
+        <v>0.150218043533832</v>
+      </c>
+      <c r="E152" t="n">
+        <v>0.880867590950911</v>
+      </c>
+      <c r="F152" t="n">
+        <v>0.968370994025505</v>
+      </c>
+      <c r="G152" t="n">
+        <v>-10.6139219590328</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>126</v>
+      </c>
+      <c r="B153" t="n">
+        <v>-0.0000202514233311681</v>
+      </c>
+      <c r="C153" t="n">
+        <v>0.0424545454545455</v>
+      </c>
+      <c r="D153" t="n">
+        <v>-0.138521664858264</v>
+      </c>
+      <c r="E153" t="n">
+        <v>0.890081326885175</v>
+      </c>
+      <c r="F153" t="n">
+        <v>0.970493444016529</v>
+      </c>
+      <c r="G153" t="n">
+        <v>-10.6156255757238</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>151</v>
+      </c>
+      <c r="B154" t="n">
+        <v>-0.0000236903442741967</v>
+      </c>
+      <c r="C154" t="n">
+        <v>0.00618181818181818</v>
+      </c>
+      <c r="D154" t="n">
+        <v>-0.132930730607274</v>
+      </c>
+      <c r="E154" t="n">
+        <v>0.894490945388729</v>
+      </c>
+      <c r="F154" t="n">
+        <v>0.970493444016529</v>
+      </c>
+      <c r="G154" t="n">
+        <v>-10.616391175281</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" t="n">
+        <v>-0.0000271292652172257</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0.0866363636363636</v>
+      </c>
+      <c r="D155" t="n">
+        <v>-0.10244004035527</v>
+      </c>
+      <c r="E155" t="n">
+        <v>0.918593847382861</v>
+      </c>
+      <c r="F155" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G155" t="n">
+        <v>-10.6200116085788</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>79</v>
+      </c>
+      <c r="B156" t="n">
+        <v>0.0000515838141454293</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0.478272727272727</v>
+      </c>
+      <c r="D156" t="n">
+        <v>0.0849705134693111</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0.932439233697177</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G156" t="n">
+        <v>-10.6216633291301</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>56</v>
+      </c>
+      <c r="B157" t="n">
+        <v>-0.0000351534140842922</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0.180909090909091</v>
+      </c>
+      <c r="D157" t="n">
+        <v>-0.084124844348072</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0.933110025236535</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G157" t="n">
+        <v>-10.6217354731413</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>38</v>
+      </c>
+      <c r="B158" t="n">
+        <v>-0.0000244545489282026</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0.813454545454545</v>
+      </c>
+      <c r="D158" t="n">
+        <v>-0.0702632579526554</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0.94411165864264</v>
+      </c>
+      <c r="F158" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G158" t="n">
+        <v>-10.622815163933</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>77</v>
+      </c>
+      <c r="B159" t="n">
+        <v>-0.0000191051163501586</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0.00709090909090909</v>
+      </c>
+      <c r="D159" t="n">
+        <v>-0.0619365599661606</v>
+      </c>
+      <c r="E159" t="n">
+        <v>0.950725710527596</v>
+      </c>
+      <c r="F159" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G159" t="n">
+        <v>-10.6233705342921</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>141</v>
+      </c>
+      <c r="B160" t="n">
+        <v>0.0000424133582973517</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0.0308181818181818</v>
+      </c>
+      <c r="D160" t="n">
+        <v>0.0573649247417911</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0.954358539332919</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G160" t="n">
+        <v>-10.6236457034118</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>71</v>
+      </c>
+      <c r="B161" t="n">
+        <v>0.0000126093767911049</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0.0675454545454545</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0.0545352190765475</v>
+      </c>
+      <c r="E161" t="n">
+        <v>0.95660763846531</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G161" t="n">
+        <v>-10.6238054589365</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>154</v>
+      </c>
+      <c r="B162" t="n">
+        <v>-0.00000649573955905395</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0.00554545454545455</v>
+      </c>
+      <c r="D162" t="n">
+        <v>-0.0433969633517654</v>
+      </c>
+      <c r="E162" t="n">
+        <v>0.965463747547613</v>
+      </c>
+      <c r="F162" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G162" t="n">
+        <v>-10.6243557967723</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>116</v>
+      </c>
+      <c r="B163" t="n">
+        <v>0.00000955255817507943</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="D163" t="n">
+        <v>0.0374807371183425</v>
+      </c>
+      <c r="E163" t="n">
+        <v>0.970169609864525</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G163" t="n">
+        <v>-10.6245972113095</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>74</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0.00000993466050208246</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0.102181818181818</v>
+      </c>
+      <c r="D164" t="n">
+        <v>0.0363057851878232</v>
+      </c>
+      <c r="E164" t="n">
+        <v>0.971104316304966</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G164" t="n">
+        <v>-10.624640952249</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>135</v>
+      </c>
+      <c r="B165" t="n">
+        <v>-0.00000382102327003171</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0.00381818181818182</v>
+      </c>
+      <c r="D165" t="n">
+        <v>-0.0282512219053665</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0.977512956962374</v>
+      </c>
+      <c r="F165" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G165" t="n">
+        <v>-10.624903300123</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>119</v>
+      </c>
+      <c r="B166" t="n">
+        <v>-0.00000420312559703503</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0.0486363636363636</v>
+      </c>
+      <c r="D166" t="n">
+        <v>-0.0235059252438312</v>
+      </c>
+      <c r="E166" t="n">
+        <v>0.981289284189697</v>
+      </c>
+      <c r="F166" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G166" t="n">
+        <v>-10.6250272161192</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>112</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.0000026747162890222</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0.0186363636363636</v>
+      </c>
+      <c r="D167" t="n">
+        <v>0.0222331542577187</v>
+      </c>
+      <c r="E167" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0.982302236597056</v>
+      </c>
+      <c r="G167" t="n">
+        <v>-10.6250565880137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="n">
+        <v>8810375</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8810412</v>
+      </c>
+      <c r="D2" t="n">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.00000000000100349979572438</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0343557533584769</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.17406936060527</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0885928348194598</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0045919285445363</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.00322576974485586</v>
+      </c>
+      <c r="M2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>

</xml_diff>